<commit_message>
fixing scale of sample chart
</commit_message>
<xml_diff>
--- a/data/samplecurves.xlsx
+++ b/data/samplecurves.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawatzd1\Documents\code\graphregression\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\www\graphcanvas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D50A422-DCA0-4F4D-AC0F-9D851F177A52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BE680E-14E5-4CB1-8243-1C90A7AA61A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C7BC972-AEFD-405E-BB58-870BC0490B7A}"/>
   </bookViews>
@@ -1133,13 +1133,13 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>133349</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>119061</xdr:rowOff>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1467,10 +1467,13 @@
   <dimension ref="H11:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="X38" sqref="X38"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="24" max="24" width="15" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="11" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H11" t="s">
@@ -1494,7 +1497,7 @@
         <v>2</v>
       </c>
       <c r="I13">
-        <f t="shared" ref="I13:I31" si="0">-0.7*H13^3+12*H13^2+5*H13+9</f>
+        <f t="shared" ref="I13:I28" si="0">-0.7*H13^3+12*H13^2+5*H13+9</f>
         <v>61.4</v>
       </c>
     </row>

</xml_diff>